<commit_message>
update table and families
</commit_message>
<xml_diff>
--- a/schema_hbase.xlsx
+++ b/schema_hbase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.lhuillier\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B59757-0FF9-4CA7-A274-2D877908A861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E2BDAA-D825-4B71-94C4-BD8C757AB5D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{78C40C59-60E3-49F1-BC2E-25ED88A9BCE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="332" xr2:uid="{78C40C59-60E3-49F1-BC2E-25ED88A9BCE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>CUSTOMER</t>
   </si>
@@ -91,6 +91,111 @@
   </si>
   <si>
     <t>key : on va générer un identifiant unique en se basant l'email (email ne peut appartenir qu'à un client)</t>
+  </si>
+  <si>
+    <t>active : permet de définir si le compte est actif ou non</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FILM</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>key1</t>
+  </si>
+  <si>
+    <t>key2</t>
+  </si>
+  <si>
+    <t>key3</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>release_year</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>movie</t>
+  </si>
+  <si>
+    <t>movie(mov)</t>
+  </si>
+  <si>
+    <t>distribution (dis)</t>
+  </si>
+  <si>
+    <t>ACTOR</t>
+  </si>
+  <si>
+    <t>families</t>
+  </si>
+  <si>
+    <t>civilitéActor(civA)</t>
+  </si>
+  <si>
+    <t>first_name_actor</t>
+  </si>
+  <si>
+    <t>last_name_actor</t>
+  </si>
+  <si>
+    <t>actor_key</t>
+  </si>
+  <si>
+    <t>actor1</t>
+  </si>
+  <si>
+    <t>actor2</t>
+  </si>
+  <si>
+    <t>actorX</t>
+  </si>
+  <si>
+    <t>langage_name</t>
+  </si>
+  <si>
+    <t>original_langage</t>
+  </si>
+  <si>
+    <t>rental_duration</t>
+  </si>
+  <si>
+    <t>Rental</t>
+  </si>
+  <si>
+    <t>rentalMovie (ren)</t>
+  </si>
+  <si>
+    <t>movieKey</t>
+  </si>
+  <si>
+    <t>rental_rate</t>
+  </si>
+  <si>
+    <t>special_features</t>
+  </si>
+  <si>
+    <t>store</t>
+  </si>
+  <si>
+    <t>storeKey</t>
+  </si>
+  <si>
+    <t>categorie</t>
+  </si>
+  <si>
+    <t>rating</t>
   </si>
 </sst>
 </file>
@@ -114,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -137,17 +242,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,22 +598,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECFC835-C618-496C-AE3D-B0D181DA523C}">
-  <dimension ref="A2:N11"/>
+  <dimension ref="A2:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -495,26 +636,30 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
@@ -524,16 +669,18 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -553,28 +700,28 @@
       <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -587,9 +734,13 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -601,9 +752,13 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -615,8 +770,10 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -629,18 +786,277 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="C16:O16"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="C2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>